<commit_message>
added: test ds for multi LR
</commit_message>
<xml_diff>
--- a/sampleData.xlsx
+++ b/sampleData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="516" yWindow="588" windowWidth="14052" windowHeight="9408" firstSheet="2" activeTab="7"/>
+    <workbookView xWindow="516" yWindow="588" windowWidth="14052" windowHeight="9408" firstSheet="2" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Drinks" sheetId="1" r:id="rId1"/>
@@ -20,13 +20,14 @@
     <sheet name="Spam" sheetId="6" r:id="rId6"/>
     <sheet name="Mouse" sheetId="7" r:id="rId7"/>
     <sheet name="Weight" sheetId="8" r:id="rId8"/>
+    <sheet name="WeightForMultiLR" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="77">
   <si>
     <t>Day</t>
   </si>
@@ -248,6 +249,15 @@
   </si>
   <si>
     <t>Weight(kg)</t>
+  </si>
+  <si>
+    <t>Weight</t>
+  </si>
+  <si>
+    <t>TailLength</t>
+  </si>
+  <si>
+    <t>Size</t>
   </si>
 </sst>
 </file>
@@ -8578,7 +8588,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
@@ -8726,4 +8736,129 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0.9</v>
+      </c>
+      <c r="B2">
+        <v>0.7</v>
+      </c>
+      <c r="C2">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1.8</v>
+      </c>
+      <c r="B3">
+        <v>1.3</v>
+      </c>
+      <c r="C3">
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2.4</v>
+      </c>
+      <c r="B4">
+        <v>0.7</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3.5</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>3.7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>3.9</v>
+      </c>
+      <c r="B6">
+        <v>3.6</v>
+      </c>
+      <c r="C6">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7">
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="B8">
+        <v>2.9</v>
+      </c>
+      <c r="C8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>5.6</v>
+      </c>
+      <c r="B9">
+        <v>3.9</v>
+      </c>
+      <c r="C9">
+        <v>4.9000000000000004</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>6.3</v>
+      </c>
+      <c r="B10">
+        <v>4</v>
+      </c>
+      <c r="C10">
+        <v>6.3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add to sampleData: ClusterTest
</commit_message>
<xml_diff>
--- a/sampleData.xlsx
+++ b/sampleData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="516" yWindow="588" windowWidth="14052" windowHeight="9408" firstSheet="3" activeTab="9"/>
+    <workbookView xWindow="516" yWindow="588" windowWidth="14052" windowHeight="9408" firstSheet="3" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Drinks" sheetId="1" r:id="rId1"/>
@@ -22,13 +22,14 @@
     <sheet name="Weight" sheetId="8" r:id="rId8"/>
     <sheet name="WeightForMultiLR" sheetId="9" r:id="rId9"/>
     <sheet name="ClusterExample" sheetId="10" r:id="rId10"/>
+    <sheet name="ClusterTest" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="114">
   <si>
     <t>Day</t>
   </si>
@@ -298,6 +299,78 @@
   </si>
   <si>
     <t>I</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Income</t>
+  </si>
+  <si>
+    <t>Bob</t>
+  </si>
+  <si>
+    <t>Michael</t>
+  </si>
+  <si>
+    <t>Mohan</t>
+  </si>
+  <si>
+    <t>Ismail</t>
+  </si>
+  <si>
+    <t>Kory</t>
+  </si>
+  <si>
+    <t>Gautam</t>
+  </si>
+  <si>
+    <t>David</t>
+  </si>
+  <si>
+    <t>Andrea</t>
+  </si>
+  <si>
+    <t>Brad</t>
+  </si>
+  <si>
+    <t>Angelina</t>
+  </si>
+  <si>
+    <t>Donald</t>
+  </si>
+  <si>
+    <t>Tom</t>
+  </si>
+  <si>
+    <t>Arnold</t>
+  </si>
+  <si>
+    <t>Jared</t>
+  </si>
+  <si>
+    <t>Stark</t>
+  </si>
+  <si>
+    <t>Ranbir</t>
+  </si>
+  <si>
+    <t>Dipika</t>
+  </si>
+  <si>
+    <t>Priyanka</t>
+  </si>
+  <si>
+    <t>Nick</t>
+  </si>
+  <si>
+    <t>Alisa</t>
+  </si>
+  <si>
+    <t>Sid</t>
+  </si>
+  <si>
+    <t>Tim</t>
   </si>
 </sst>
 </file>
@@ -4666,7 +4739,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -4791,6 +4864,274 @@
       </c>
       <c r="C11">
         <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2">
+        <v>27</v>
+      </c>
+      <c r="C2">
+        <v>70000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B3">
+        <v>29</v>
+      </c>
+      <c r="C3">
+        <v>90000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B4">
+        <v>29</v>
+      </c>
+      <c r="C4">
+        <v>61000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>95</v>
+      </c>
+      <c r="B5">
+        <v>28</v>
+      </c>
+      <c r="C5">
+        <v>60000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>96</v>
+      </c>
+      <c r="B6">
+        <v>42</v>
+      </c>
+      <c r="C6">
+        <v>150000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B7">
+        <v>39</v>
+      </c>
+      <c r="C7">
+        <v>155000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>98</v>
+      </c>
+      <c r="B8">
+        <v>41</v>
+      </c>
+      <c r="C8">
+        <v>160000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>99</v>
+      </c>
+      <c r="B9">
+        <v>38</v>
+      </c>
+      <c r="C9">
+        <v>162000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>100</v>
+      </c>
+      <c r="B10">
+        <v>36</v>
+      </c>
+      <c r="C10">
+        <v>156000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>101</v>
+      </c>
+      <c r="B11">
+        <v>35</v>
+      </c>
+      <c r="C11">
+        <v>130000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>102</v>
+      </c>
+      <c r="B12">
+        <v>37</v>
+      </c>
+      <c r="C12">
+        <v>137000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>103</v>
+      </c>
+      <c r="B13">
+        <v>26</v>
+      </c>
+      <c r="C13">
+        <v>45000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>104</v>
+      </c>
+      <c r="B14">
+        <v>27</v>
+      </c>
+      <c r="C14">
+        <v>48000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>105</v>
+      </c>
+      <c r="B15">
+        <v>28</v>
+      </c>
+      <c r="C15">
+        <v>51000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>106</v>
+      </c>
+      <c r="B16">
+        <v>29</v>
+      </c>
+      <c r="C16">
+        <v>49500</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>107</v>
+      </c>
+      <c r="B17">
+        <v>32</v>
+      </c>
+      <c r="C17">
+        <v>53000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>108</v>
+      </c>
+      <c r="B18">
+        <v>40</v>
+      </c>
+      <c r="C18">
+        <v>65000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>109</v>
+      </c>
+      <c r="B19">
+        <v>41</v>
+      </c>
+      <c r="C19">
+        <v>63000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>110</v>
+      </c>
+      <c r="B20">
+        <v>43</v>
+      </c>
+      <c r="C20">
+        <v>64000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>111</v>
+      </c>
+      <c r="B21">
+        <v>39</v>
+      </c>
+      <c r="C21">
+        <v>80000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>112</v>
+      </c>
+      <c r="B22">
+        <v>41</v>
+      </c>
+      <c r="C22">
+        <v>82000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>113</v>
+      </c>
+      <c r="B23">
+        <v>39</v>
+      </c>
+      <c r="C23">
+        <v>58000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>